<commit_message>
Update IP - EX 29 - Congelar, dividir paineis e agrupamento (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 29 - Congelar, dividir paineis e agrupamento (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 29 - Congelar, dividir paineis e agrupamento (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1A3117-BA3B-4BF7-8454-BA5AFB5C4D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8543DCD0-15D2-4773-949A-AE90FE5F1EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -1119,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1305,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G618"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>